<commit_message>
Better description of labs
</commit_message>
<xml_diff>
--- a/assets/database.xlsx
+++ b/assets/database.xlsx
@@ -81,25 +81,7 @@
     <t xml:space="preserve">https://ui.adsabs.harvard.edu/abs/2021AGUFM.H35A..08S/abstract</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Ubuntu"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://agu2021fallmeeting</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Ubuntu"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">-agu.ipostersessions.com/Default.aspx?s=7C-2F-8F-99-C9-B5-36-0A-29-6A-62-35-E4-87-05-80</t>
-    </r>
+    <t xml:space="preserve">https://agu2021fallmeeting-agu.ipostersessions.com/Default.aspx?s=7C-2F-8F-99-C9-B5-36-0A-29-6A-62-35-E4-87-05-80</t>
   </si>
   <si>
     <t xml:space="preserve">https://docs.google.com/presentation/d/1Jar5ThSvhYYakgkJcQerM6tUsDkK27dI7FHSKAOGxEs/edit?usp=sharing</t>
@@ -120,25 +102,7 @@
     <t xml:space="preserve">https://ui.adsabs.harvard.edu/abs/2020AGUFMH112.0022S/abstract</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Ubuntu"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://agu2020fallmeeting</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Ubuntu"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">-agu.ipostersessions.com/Default.aspx?s=62-6F-B7-67-7E-99-AB-5C-EF-80-72-EF-68-3B-1D-93</t>
-    </r>
+    <t xml:space="preserve">https://agu2020fallmeeting-agu.ipostersessions.com/Default.aspx?s=62-6F-B7-67-7E-99-AB-5C-EF-80-72-EF-68-3B-1D-93</t>
   </si>
   <si>
     <t xml:space="preserve">https://docs.google.com/presentation/d/1M4uneQHBRlifLg2tcduoXKDNR0qy_G_FC06FYR3oAU8/edit?usp=sharing</t>
@@ -174,7 +138,7 @@
     <t xml:space="preserve">Turbulence and open channel flow</t>
   </si>
   <si>
-    <t xml:space="preserve">Gather high-resolution velocity readings and quantify turbulence features</t>
+    <t xml:space="preserve">Gather high-resolution velocity data of an open channel flow to quantify its turbulence characteristics.</t>
   </si>
   <si>
     <t xml:space="preserve">cee440-lab1.png</t>
@@ -192,7 +156,7 @@
     <t xml:space="preserve">Sediment flux and bedform migration</t>
   </si>
   <si>
-    <t xml:space="preserve">Capture time-lapse of bed sediment motion and calculate morphodynamic parameters</t>
+    <t xml:space="preserve">Capture timelapse imagery of bed sediment motion to calculate morphodynamic parameters.</t>
   </si>
   <si>
     <t xml:space="preserve">cee440-lab2.png</t>
@@ -258,6 +222,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -292,6 +257,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -370,7 +336,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -380,13 +346,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.58"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="112.1"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="112.12"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -408,7 +374,7 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -454,7 +420,7 @@
       <c r="F3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -468,7 +434,7 @@
       <c r="C4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -509,8 +475,8 @@
     <hyperlink ref="E2" r:id="rId1" display="https://drive.google.com/file/d/1n4LyC7PC8ML3Ny5RyEXh2dLLz_p2_1hj/view?usp=sharing"/>
     <hyperlink ref="G2" r:id="rId2" display="https://drive.google.com/file/d/1mWvkKyYLSsTlcwhARnBcJIzybApNEjBO/view?usp=sharing"/>
     <hyperlink ref="E3" r:id="rId3" display="https://ui.adsabs.harvard.edu/abs/2021AGUFM.H35A..08S/abstract"/>
-    <hyperlink ref="F3" r:id="rId4" display="https://agu2021fallmeeting"/>
-    <hyperlink ref="F4" r:id="rId5" display="https://agu2020fallmeeting"/>
+    <hyperlink ref="F3" r:id="rId4" display="https://agu2021fallmeeting-agu.ipostersessions.com/Default.aspx?s=7C-2F-8F-99-C9-B5-36-0A-29-6A-62-35-E4-87-05-80"/>
+    <hyperlink ref="F4" r:id="rId5" display="https://agu2020fallmeeting-agu.ipostersessions.com/Default.aspx?s=62-6F-B7-67-7E-99-AB-5C-EF-80-72-EF-68-3B-1D-93"/>
     <hyperlink ref="G4" r:id="rId6" display="https://docs.google.com/presentation/d/1M4uneQHBRlifLg2tcduoXKDNR0qy_G_FC06FYR3oAU8/edit?usp=sharing"/>
     <hyperlink ref="E5" r:id="rId7" display="https://www.iahr.org/library/infor?pid=2780"/>
     <hyperlink ref="F5" r:id="rId8" display="https://docs.google.com/presentation/d/19FHSVl-1zOyDizwIS_TKlSMjRn4btvFn/edit?usp=sharing&amp;ouid=100415341907401448709&amp;rtpof=true&amp;sd=true"/>
@@ -518,7 +484,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -527,17 +493,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="72.81"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -555,24 +525,24 @@
       <c r="E1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -580,16 +550,16 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -607,7 +577,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -616,7 +586,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -626,7 +596,7 @@
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -638,24 +608,24 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -664,18 +634,18 @@
       <c r="E2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>58</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -684,7 +654,7 @@
       <c r="E3" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="2" t="s">
         <v>61</v>
       </c>
     </row>
@@ -697,7 +667,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>